<commit_message>
modify investor profit flow report template
</commit_message>
<xml_diff>
--- a/src/Presentation/CTM.Win/ReportTemplate/UserDailyProfitFlow/TargetReport.xlsx
+++ b/src/Presentation/CTM.Win/ReportTemplate/UserDailyProfitFlow/TargetReport.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-30" yWindow="1050" windowWidth="18825" windowHeight="6780" tabRatio="693"/>
@@ -11,7 +11,7 @@
     <sheet name="合计" sheetId="177" r:id="rId2"/>
     <sheet name="吴强" sheetId="180" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -955,8 +955,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="83387520"/>
-        <c:axId val="83389056"/>
+        <c:axId val="-852933888"/>
+        <c:axId val="-852944224"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2069,8 +2069,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="83387520"/>
-        <c:axId val="83389056"/>
+        <c:axId val="-852933888"/>
+        <c:axId val="-852944224"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2961,11 +2961,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="83392768"/>
-        <c:axId val="83391232"/>
+        <c:axId val="-852944768"/>
+        <c:axId val="-852952928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="83387520"/>
+        <c:axId val="-852933888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2985,7 +2985,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83389056"/>
+        <c:crossAx val="-852944224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -2993,7 +2993,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83389056"/>
+        <c:axId val="-852944224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3065,12 +3065,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83387520"/>
+        <c:crossAx val="-852933888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="83391232"/>
+        <c:axId val="-852952928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3090,12 +3090,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83392768"/>
+        <c:crossAx val="-852944768"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="83392768"/>
+        <c:axId val="-852944768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3104,7 +3104,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83391232"/>
+        <c:crossAx val="-852952928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3721,8 +3721,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="83555072"/>
-        <c:axId val="83556608"/>
+        <c:axId val="-852926816"/>
+        <c:axId val="-852940416"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -4835,8 +4835,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="83555072"/>
-        <c:axId val="83556608"/>
+        <c:axId val="-852926816"/>
+        <c:axId val="-852940416"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -5727,11 +5727,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="83625856"/>
-        <c:axId val="83624320"/>
+        <c:axId val="-852955104"/>
+        <c:axId val="-852955648"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="83555072"/>
+        <c:axId val="-852926816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5751,7 +5751,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83556608"/>
+        <c:crossAx val="-852940416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -5759,7 +5759,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83556608"/>
+        <c:axId val="-852940416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5831,12 +5831,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83555072"/>
+        <c:crossAx val="-852926816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="83624320"/>
+        <c:axId val="-852955648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5856,12 +5856,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83625856"/>
+        <c:crossAx val="-852955104"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="83625856"/>
+        <c:axId val="-852955104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5870,7 +5870,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83624320"/>
+        <c:crossAx val="-852955648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6487,8 +6487,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="-68"/>
-        <c:axId val="90047616"/>
-        <c:axId val="90049152"/>
+        <c:axId val="-852943680"/>
+        <c:axId val="-852937152"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -7591,8 +7591,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="90047616"/>
-        <c:axId val="90049152"/>
+        <c:axId val="-852943680"/>
+        <c:axId val="-852937152"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -8473,11 +8473,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="90052864"/>
-        <c:axId val="90051328"/>
+        <c:axId val="-852939872"/>
+        <c:axId val="-852939328"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="90047616"/>
+        <c:axId val="-852943680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8497,7 +8497,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="90049152"/>
+        <c:crossAx val="-852937152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -8505,7 +8505,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="90049152"/>
+        <c:axId val="-852937152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8577,12 +8577,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="90047616"/>
+        <c:crossAx val="-852943680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="90051328"/>
+        <c:axId val="-852939328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8602,12 +8602,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="90052864"/>
+        <c:crossAx val="-852939872"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="90052864"/>
+        <c:axId val="-852939872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8616,7 +8616,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90051328"/>
+        <c:crossAx val="-852939328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9233,8 +9233,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="-68"/>
-        <c:axId val="90306048"/>
-        <c:axId val="90307584"/>
+        <c:axId val="-852925728"/>
+        <c:axId val="-852948032"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -10337,8 +10337,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="90306048"/>
-        <c:axId val="90307584"/>
+        <c:axId val="-852925728"/>
+        <c:axId val="-852948032"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -11219,11 +11219,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="91695744"/>
-        <c:axId val="91694208"/>
+        <c:axId val="-852949120"/>
+        <c:axId val="-852950208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="90306048"/>
+        <c:axId val="-852925728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11243,7 +11243,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="90307584"/>
+        <c:crossAx val="-852948032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -11251,7 +11251,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="90307584"/>
+        <c:axId val="-852948032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11323,12 +11323,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="90306048"/>
+        <c:crossAx val="-852925728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="91694208"/>
+        <c:axId val="-852950208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11348,12 +11348,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91695744"/>
+        <c:crossAx val="-852949120"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="91695744"/>
+        <c:axId val="-852949120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11362,7 +11362,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91694208"/>
+        <c:crossAx val="-852950208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11947,7 +11947,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -11989,7 +11989,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -12024,7 +12024,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -12235,8 +12235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A13:A94"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="T74" sqref="T74"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -12255,7 +12255,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Y65"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K59" sqref="K59"/>
     </sheetView>
   </sheetViews>
@@ -14474,7 +14474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Y65"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>

</xml_diff>